<commit_message>
(SS) Looking at I_y and CMalpha values
</commit_message>
<xml_diff>
--- a/SpaceFLight/JavaFoil_MainWingData.xlsx
+++ b/SpaceFLight/JavaFoil_MainWingData.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\CourseworkTest_Git\trunk\SpaceFLight\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Main_Wing" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>α</t>
   </si>
@@ -59,12 +64,15 @@
   <si>
     <t>CLALPHA</t>
   </si>
+  <si>
+    <t>CMALPHA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +121,1124 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Main_Wing!$A$2:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Main_Wing!$D$2:$D$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>-5.8999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-6.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-6.2E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-6.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-6.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-6.5000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-6.6000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-6.6000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-6.7000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-6.7000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-6.8000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-6.8000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-6.9000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-7.0999999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-7.1999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-7.2999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-7.2999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-7.3999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-7.3999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-7.3999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-7.3999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-4.2999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.04</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-3.9E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-3.6999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-3.6999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-3.6999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-3.6999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-3.5999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-3.5000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-3.5000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-3.5000000000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5823-4B49-A29E-7205E03350A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="507208216"/>
+        <c:axId val="507209528"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="507208216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="507209528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="507209528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="507208216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,27 +1496,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -430,8 +1556,11 @@
       <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -470,11 +1599,14 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <f>(B23-B2)/(M23-M2)</f>
-        <v>4.8728696290650007</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <f>(B22-B2)/(M22-M2)</f>
+        <v>4.9732736617355453</v>
+      </c>
+      <c r="P2">
+        <v>-0.68300000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.5</v>
       </c>
@@ -513,7 +1645,7 @@
         <v>8.7266462599716477E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -552,7 +1684,7 @@
         <v>1.7453292519943295E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1.5</v>
       </c>
@@ -591,7 +1723,7 @@
         <v>2.6179938779914945E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -630,7 +1762,7 @@
         <v>3.4906585039886591E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2.5</v>
       </c>
@@ -669,7 +1801,7 @@
         <v>4.3633231299858237E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -708,7 +1840,7 @@
         <v>5.235987755982989E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3.5</v>
       </c>
@@ -747,7 +1879,7 @@
         <v>6.1086523819801536E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -786,7 +1918,7 @@
         <v>6.9813170079773182E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>4.5</v>
       </c>
@@ -825,7 +1957,7 @@
         <v>7.8539816339744828E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -864,7 +1996,7 @@
         <v>8.7266462599716474E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>5.5</v>
       </c>
@@ -903,7 +2035,7 @@
         <v>9.599310885968812E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>6</v>
       </c>
@@ -942,7 +2074,7 @@
         <v>0.10471975511965978</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>6.5</v>
       </c>
@@ -981,7 +2113,7 @@
         <v>0.11344640137963143</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>7</v>
       </c>
@@ -1020,7 +2152,7 @@
         <v>0.12217304763960307</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>7.5</v>
       </c>
@@ -1059,7 +2191,7 @@
         <v>0.1308996938995747</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>8</v>
       </c>
@@ -1098,7 +2230,7 @@
         <v>0.13962634015954636</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>8.5</v>
       </c>
@@ -1137,7 +2269,7 @@
         <v>0.14835298641951802</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>9</v>
       </c>
@@ -1176,7 +2308,7 @@
         <v>0.15707963267948966</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>9.5</v>
       </c>
@@ -1215,7 +2347,7 @@
         <v>0.16580627893946132</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>10</v>
       </c>
@@ -1254,7 +2386,7 @@
         <v>0.17453292519943295</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>10.5</v>
       </c>
@@ -1293,7 +2425,7 @@
         <v>0.18325957145940461</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>11</v>
       </c>
@@ -1332,7 +2464,7 @@
         <v>0.19198621771937624</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>11.5</v>
       </c>
@@ -1371,7 +2503,7 @@
         <v>0.2007128639793479</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>12</v>
       </c>
@@ -1410,7 +2542,7 @@
         <v>0.20943951023931956</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>12.5</v>
       </c>
@@ -1449,7 +2581,7 @@
         <v>0.21816615649929119</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>13</v>
       </c>
@@ -1488,7 +2620,7 @@
         <v>0.22689280275926285</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>13.5</v>
       </c>
@@ -1527,7 +2659,7 @@
         <v>0.23561944901923448</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>14</v>
       </c>
@@ -1566,7 +2698,7 @@
         <v>0.24434609527920614</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>14.5</v>
       </c>
@@ -1605,7 +2737,7 @@
         <v>0.2530727415391778</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>15</v>
       </c>
@@ -1644,7 +2776,7 @@
         <v>0.26179938779914941</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>15.5</v>
       </c>
@@ -1683,7 +2815,7 @@
         <v>0.27052603405912107</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>16</v>
       </c>
@@ -1722,7 +2854,7 @@
         <v>0.27925268031909273</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>16.5</v>
       </c>
@@ -1761,7 +2893,7 @@
         <v>0.28797932657906439</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>17</v>
       </c>
@@ -1800,7 +2932,7 @@
         <v>0.29670597283903605</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>17.5</v>
       </c>
@@ -1839,7 +2971,7 @@
         <v>0.30543261909900765</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>18</v>
       </c>
@@ -1878,7 +3010,7 @@
         <v>0.31415926535897931</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>18.5</v>
       </c>
@@ -1917,7 +3049,7 @@
         <v>0.32288591161895097</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>19</v>
       </c>
@@ -1956,7 +3088,7 @@
         <v>0.33161255787892263</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>19.5</v>
       </c>
@@ -1995,7 +3127,7 @@
         <v>0.34033920413889424</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>20</v>
       </c>
@@ -2037,5 +3169,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>